<commit_message>
updated 2024 plate 3 map
</commit_message>
<xml_diff>
--- a/data/AY2024_JGI_plate03_map.xlsx
+++ b/data/AY2024_JGI_plate03_map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/crossh/repos/nmdc_microbe/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{236DC428-364B-FF49-BF43-F4228949661F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{702D0533-F760-374E-9CE0-35A37674D256}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13980" yWindow="2120" windowWidth="31020" windowHeight="23940" xr2:uid="{90ABCA6C-197C-6F4D-BB0A-1C7CB343162A}"/>
+    <workbookView xWindow="0" yWindow="700" windowWidth="27040" windowHeight="15460" xr2:uid="{90ABCA6C-197C-6F4D-BB0A-1C7CB343162A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="327">
   <si>
     <t>dnaSampleID</t>
   </si>
@@ -1014,6 +1014,9 @@
   </si>
   <si>
     <t>24S_33_3028</t>
+  </si>
+  <si>
+    <t>more DNA needed for this sample</t>
   </si>
 </sst>
 </file>
@@ -1066,7 +1069,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1097,6 +1100,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1132,7 +1141,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1155,7 +1164,8 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="3"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="60% - Accent5" xfId="4" builtinId="48"/>
@@ -1497,7 +1507,7 @@
   <dimension ref="A1:H97"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D74" sqref="D74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1565,6 +1575,9 @@
       <c r="F3" s="4" t="s">
         <v>9</v>
       </c>
+      <c r="G3">
+        <v>30</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -1585,6 +1598,9 @@
       <c r="F4" s="5" t="s">
         <v>10</v>
       </c>
+      <c r="G4">
+        <v>30</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -1605,6 +1621,9 @@
       <c r="F5" s="5" t="s">
         <v>11</v>
       </c>
+      <c r="G5">
+        <v>30</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -1625,6 +1644,9 @@
       <c r="F6" s="5" t="s">
         <v>12</v>
       </c>
+      <c r="G6">
+        <v>30</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -1645,6 +1667,9 @@
       <c r="F7" s="5" t="s">
         <v>13</v>
       </c>
+      <c r="G7">
+        <v>30</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -1665,6 +1690,9 @@
       <c r="F8" s="5" t="s">
         <v>14</v>
       </c>
+      <c r="G8">
+        <v>30</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
@@ -1693,6 +1721,9 @@
       <c r="F10" s="6" t="s">
         <v>16</v>
       </c>
+      <c r="G10">
+        <v>30</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -1713,6 +1744,9 @@
       <c r="F11" s="7" t="s">
         <v>17</v>
       </c>
+      <c r="G11">
+        <v>30</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -1733,6 +1767,9 @@
       <c r="F12" s="6" t="s">
         <v>18</v>
       </c>
+      <c r="G12">
+        <v>30</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -1753,6 +1790,9 @@
       <c r="F13" s="6" t="s">
         <v>19</v>
       </c>
+      <c r="G13">
+        <v>30</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -1773,6 +1813,9 @@
       <c r="F14" s="6" t="s">
         <v>20</v>
       </c>
+      <c r="G14">
+        <v>30</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
@@ -1793,6 +1836,9 @@
       <c r="F15" s="6" t="s">
         <v>21</v>
       </c>
+      <c r="G15">
+        <v>30</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
@@ -1813,8 +1859,11 @@
       <c r="F16" s="6" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G16">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>185</v>
       </c>
@@ -1833,8 +1882,11 @@
       <c r="F17" s="7" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G17">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>187</v>
       </c>
@@ -1853,8 +1905,11 @@
       <c r="F18" s="5" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G18">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>189</v>
       </c>
@@ -1873,8 +1928,11 @@
       <c r="F19" s="5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G19">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>191</v>
       </c>
@@ -1893,28 +1951,37 @@
       <c r="F20" s="5" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G20">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>194</v>
       </c>
       <c r="B21" t="s">
         <v>195</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="11">
         <v>12</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="11" t="s">
         <v>168</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="11" t="s">
         <v>196</v>
       </c>
       <c r="F21" s="5" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G21" s="11">
+        <v>50</v>
+      </c>
+      <c r="H21" s="10" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>197</v>
       </c>
@@ -1933,8 +2000,11 @@
       <c r="F22" s="5" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G22">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>200</v>
       </c>
@@ -1953,8 +2023,11 @@
       <c r="F23" s="5" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G23">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>203</v>
       </c>
@@ -1973,8 +2046,11 @@
       <c r="F24" s="5" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G24">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>205</v>
       </c>
@@ -1993,8 +2069,11 @@
       <c r="F25" s="5" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>207</v>
       </c>
@@ -2013,8 +2092,11 @@
       <c r="F26" s="6" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G26">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>209</v>
       </c>
@@ -2033,8 +2115,11 @@
       <c r="F27" s="6" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G27">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>211</v>
       </c>
@@ -2053,8 +2138,11 @@
       <c r="F28" s="6" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G28">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>213</v>
       </c>
@@ -2073,8 +2161,11 @@
       <c r="F29" s="7" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G29">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>215</v>
       </c>
@@ -2093,8 +2184,11 @@
       <c r="F30" s="6" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G30">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>217</v>
       </c>
@@ -2113,8 +2207,11 @@
       <c r="F31" s="6" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G31">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>220</v>
       </c>
@@ -2133,8 +2230,11 @@
       <c r="F32" s="6" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G32">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>222</v>
       </c>
@@ -2153,8 +2253,11 @@
       <c r="F33" s="6" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G33">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>224</v>
       </c>
@@ -2173,8 +2276,11 @@
       <c r="F34" s="5" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G34">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>226</v>
       </c>
@@ -2193,8 +2299,11 @@
       <c r="F35" s="5" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G35">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>228</v>
       </c>
@@ -2213,8 +2322,11 @@
       <c r="F36" s="5" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G36">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>230</v>
       </c>
@@ -2233,8 +2345,11 @@
       <c r="F37" s="5" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G37">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>232</v>
       </c>
@@ -2253,8 +2368,11 @@
       <c r="F38" s="5" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G38">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>235</v>
       </c>
@@ -2273,28 +2391,37 @@
       <c r="F39" s="5" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G39">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>238</v>
       </c>
       <c r="B40" t="s">
         <v>239</v>
       </c>
-      <c r="C40">
+      <c r="C40" s="11">
         <v>12</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D40" s="11" t="s">
         <v>234</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E40" s="11" t="s">
         <v>116</v>
       </c>
       <c r="F40" s="4" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G40" s="11">
+        <v>50</v>
+      </c>
+      <c r="H40" s="10" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>240</v>
       </c>
@@ -2313,8 +2440,11 @@
       <c r="F41" s="5" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G41">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>242</v>
       </c>
@@ -2333,8 +2463,11 @@
       <c r="F42" s="6" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G42">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>245</v>
       </c>
@@ -2353,8 +2486,11 @@
       <c r="F43" s="6" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G43">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>248</v>
       </c>
@@ -2373,8 +2509,11 @@
       <c r="F44" s="6" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G44">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>250</v>
       </c>
@@ -2393,8 +2532,11 @@
       <c r="F45" s="6" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G45">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>252</v>
       </c>
@@ -2413,28 +2555,37 @@
       <c r="F46" s="6" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G46">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>254</v>
       </c>
       <c r="B47" t="s">
         <v>255</v>
       </c>
-      <c r="C47">
+      <c r="C47" s="11">
         <v>17</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D47" s="11" t="s">
         <v>234</v>
       </c>
-      <c r="E47" t="s">
+      <c r="E47" s="11" t="s">
         <v>122</v>
       </c>
       <c r="F47" s="6" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G47" s="11">
+        <v>50</v>
+      </c>
+      <c r="H47" s="10" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>256</v>
       </c>
@@ -2452,6 +2603,9 @@
       </c>
       <c r="F48" s="6" t="s">
         <v>54</v>
+      </c>
+      <c r="G48">
+        <v>30</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
@@ -2473,6 +2627,9 @@
       <c r="F49" s="6" t="s">
         <v>55</v>
       </c>
+      <c r="G49">
+        <v>30</v>
+      </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
@@ -2493,6 +2650,9 @@
       <c r="F50" s="5" t="s">
         <v>56</v>
       </c>
+      <c r="G50">
+        <v>30</v>
+      </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
@@ -2513,6 +2673,9 @@
       <c r="F51" s="5" t="s">
         <v>57</v>
       </c>
+      <c r="G51">
+        <v>30</v>
+      </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
@@ -2533,6 +2696,9 @@
       <c r="F52" s="5" t="s">
         <v>58</v>
       </c>
+      <c r="G52">
+        <v>30</v>
+      </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
@@ -2553,6 +2719,9 @@
       <c r="F53" s="5" t="s">
         <v>59</v>
       </c>
+      <c r="G53">
+        <v>30</v>
+      </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
@@ -2573,6 +2742,9 @@
       <c r="F54" s="5" t="s">
         <v>60</v>
       </c>
+      <c r="G54">
+        <v>30</v>
+      </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
@@ -2593,6 +2765,9 @@
       <c r="F55" s="5" t="s">
         <v>61</v>
       </c>
+      <c r="G55">
+        <v>30</v>
+      </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
@@ -2613,7 +2788,9 @@
       <c r="F56" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="G56" s="9"/>
+      <c r="G56">
+        <v>30</v>
+      </c>
       <c r="H56" s="9"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
@@ -2635,8 +2812,9 @@
       <c r="F57" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="G57" s="10"/>
-      <c r="H57" s="10"/>
+      <c r="G57">
+        <v>30</v>
+      </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
@@ -2657,8 +2835,9 @@
       <c r="F58" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="G58" s="10"/>
-      <c r="H58" s="10"/>
+      <c r="G58">
+        <v>30</v>
+      </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
@@ -2679,8 +2858,9 @@
       <c r="F59" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="G59" s="10"/>
-      <c r="H59" s="10"/>
+      <c r="G59">
+        <v>30</v>
+      </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
@@ -2689,20 +2869,24 @@
       <c r="B60" t="s">
         <v>284</v>
       </c>
-      <c r="C60">
+      <c r="C60" s="11">
         <v>10</v>
       </c>
-      <c r="D60" t="s">
+      <c r="D60" s="11" t="s">
         <v>280</v>
       </c>
-      <c r="E60" t="s">
+      <c r="E60" s="11" t="s">
         <v>130</v>
       </c>
       <c r="F60" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="G60" s="10"/>
-      <c r="H60" s="10"/>
+      <c r="G60" s="11">
+        <v>50</v>
+      </c>
+      <c r="H60" s="10" t="s">
+        <v>326</v>
+      </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
@@ -2723,8 +2907,9 @@
       <c r="F61" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="G61" s="10"/>
-      <c r="H61" s="10"/>
+      <c r="G61">
+        <v>30</v>
+      </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
@@ -2745,8 +2930,9 @@
       <c r="F62" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="G62" s="10"/>
-      <c r="H62" s="10"/>
+      <c r="G62">
+        <v>30</v>
+      </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
@@ -2767,7 +2953,9 @@
       <c r="F63" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="G63" s="9"/>
+      <c r="G63">
+        <v>30</v>
+      </c>
       <c r="H63" s="9"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
@@ -2777,20 +2965,24 @@
       <c r="B64" t="s">
         <v>292</v>
       </c>
-      <c r="C64">
+      <c r="C64" s="11">
         <v>12</v>
       </c>
-      <c r="D64" t="s">
+      <c r="D64" s="11" t="s">
         <v>280</v>
       </c>
-      <c r="E64" t="s">
+      <c r="E64" s="11" t="s">
         <v>134</v>
       </c>
       <c r="F64" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="G64" s="10"/>
-      <c r="H64" s="10"/>
+      <c r="G64" s="11">
+        <v>50</v>
+      </c>
+      <c r="H64" s="10" t="s">
+        <v>326</v>
+      </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
@@ -2799,20 +2991,24 @@
       <c r="B65" t="s">
         <v>294</v>
       </c>
-      <c r="C65">
+      <c r="C65" s="11">
         <v>15</v>
       </c>
-      <c r="D65" t="s">
+      <c r="D65" s="11" t="s">
         <v>280</v>
       </c>
-      <c r="E65" t="s">
+      <c r="E65" s="11" t="s">
         <v>135</v>
       </c>
       <c r="F65" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="G65" s="10"/>
-      <c r="H65" s="10"/>
+      <c r="G65" s="11">
+        <v>50</v>
+      </c>
+      <c r="H65" s="10" t="s">
+        <v>326</v>
+      </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
@@ -2821,20 +3017,24 @@
       <c r="B66" t="s">
         <v>296</v>
       </c>
-      <c r="C66">
+      <c r="C66" s="11">
         <v>11</v>
       </c>
-      <c r="D66" t="s">
+      <c r="D66" s="11" t="s">
         <v>280</v>
       </c>
-      <c r="E66" t="s">
+      <c r="E66" s="11" t="s">
         <v>149</v>
       </c>
       <c r="F66" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="G66" s="9"/>
-      <c r="H66" s="9"/>
+      <c r="G66" s="11">
+        <v>50</v>
+      </c>
+      <c r="H66" s="10" t="s">
+        <v>326</v>
+      </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
@@ -2855,6 +3055,9 @@
       <c r="F67" s="5" t="s">
         <v>73</v>
       </c>
+      <c r="G67">
+        <v>30</v>
+      </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
@@ -2875,6 +3078,9 @@
       <c r="F68" s="5" t="s">
         <v>74</v>
       </c>
+      <c r="G68">
+        <v>30</v>
+      </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
@@ -2883,17 +3089,23 @@
       <c r="B69" t="s">
         <v>302</v>
       </c>
-      <c r="C69">
+      <c r="C69" s="11">
         <v>15</v>
       </c>
-      <c r="D69" t="s">
+      <c r="D69" s="11" t="s">
         <v>280</v>
       </c>
-      <c r="E69" t="s">
+      <c r="E69" s="11" t="s">
         <v>152</v>
       </c>
       <c r="F69" s="5" t="s">
         <v>75</v>
+      </c>
+      <c r="G69" s="11">
+        <v>50</v>
+      </c>
+      <c r="H69" s="10" t="s">
+        <v>326</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
@@ -2903,17 +3115,23 @@
       <c r="B70" t="s">
         <v>304</v>
       </c>
-      <c r="C70">
+      <c r="C70" s="11">
         <v>18</v>
       </c>
-      <c r="D70" t="s">
+      <c r="D70" s="11" t="s">
         <v>280</v>
       </c>
-      <c r="E70" t="s">
+      <c r="E70" s="11" t="s">
         <v>153</v>
       </c>
       <c r="F70" s="5" t="s">
         <v>76</v>
+      </c>
+      <c r="G70" s="11">
+        <v>50</v>
+      </c>
+      <c r="H70" s="10" t="s">
+        <v>326</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
@@ -2935,6 +3153,9 @@
       <c r="F71" s="5" t="s">
         <v>77</v>
       </c>
+      <c r="G71">
+        <v>30</v>
+      </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
@@ -2955,6 +3176,9 @@
       <c r="F72" s="5" t="s">
         <v>78</v>
       </c>
+      <c r="G72">
+        <v>30</v>
+      </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
@@ -2975,6 +3199,9 @@
       <c r="F73" s="5" t="s">
         <v>79</v>
       </c>
+      <c r="G73">
+        <v>30</v>
+      </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
@@ -2995,6 +3222,9 @@
       <c r="F74" s="6" t="s">
         <v>80</v>
       </c>
+      <c r="G74">
+        <v>30</v>
+      </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
@@ -3015,6 +3245,9 @@
       <c r="F75" s="6" t="s">
         <v>81</v>
       </c>
+      <c r="G75">
+        <v>30</v>
+      </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
@@ -3035,6 +3268,9 @@
       <c r="F76" s="6" t="s">
         <v>82</v>
       </c>
+      <c r="G76">
+        <v>30</v>
+      </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
@@ -3055,6 +3291,9 @@
       <c r="F77" s="6" t="s">
         <v>83</v>
       </c>
+      <c r="G77">
+        <v>30</v>
+      </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
@@ -3075,6 +3314,9 @@
       <c r="F78" s="7" t="s">
         <v>84</v>
       </c>
+      <c r="G78">
+        <v>30</v>
+      </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
@@ -3095,6 +3337,9 @@
       <c r="F79" s="6" t="s">
         <v>85</v>
       </c>
+      <c r="G79">
+        <v>30</v>
+      </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F80" s="6" t="s">
@@ -3112,7 +3357,6 @@
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C83" s="10"/>
       <c r="F83" s="5" t="s">
         <v>89</v>
       </c>

</xml_diff>